<commit_message>
220606 datasets fed into pipeline
</commit_message>
<xml_diff>
--- a/data/_input/base_smartsheet.xlsx
+++ b/data/_input/base_smartsheet.xlsx
@@ -56871,13 +56871,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1715B57E-1030-48F8-9EE0-1DAB6A03C4C7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA1FD436-7066-4852-8E82-909009D86017}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10EB01A7-5FEF-41F6-AB65-33675BDDC801}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2B2F1B6-E305-4F7A-85F1-BC85721F8274}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{123C9D12-8E1A-4AD3-AF3C-541EBD84AAF1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5B7BD8-4B66-403F-994E-46EB5240163E}"/>
 </file>
</xml_diff>

<commit_message>
Data input files fo week of 220613 updated.
</commit_message>
<xml_diff>
--- a/data/_input/base_smartsheet.xlsx
+++ b/data/_input/base_smartsheet.xlsx
@@ -56864,20 +56864,10 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA1FD436-7066-4852-8E82-909009D86017}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83A233C7-E547-483C-8F50-9444D922CD1C}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2B2F1B6-E305-4F7A-85F1-BC85721F8274}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E5B7BD8-4B66-403F-994E-46EB5240163E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A3FD982-2C21-48AC-B2D6-389206791392}"/>
 </file>
</xml_diff>

<commit_message>
Latest updates - including target boosters
</commit_message>
<xml_diff>
--- a/data/_input/base_smartsheet.xlsx
+++ b/data/_input/base_smartsheet.xlsx
@@ -56865,9 +56865,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83A233C7-E547-483C-8F50-9444D922CD1C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A2179FD-40A7-466A-AC34-DA509D54BC1A}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A3FD982-2C21-48AC-B2D6-389206791392}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63D9028A-A792-4568-89FB-834F94CC1066}"/>
 </file>
</xml_diff>

<commit_message>
Modified data cleaning file & changed Kosovo's iso code
</commit_message>
<xml_diff>
--- a/data/_input/base_smartsheet.xlsx
+++ b/data/_input/base_smartsheet.xlsx
@@ -56864,20 +56864,10 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1715B57E-1030-48F8-9EE0-1DAB6A03C4C7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9D2FDD-61F1-44F5-AA71-49A169837CE8}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10EB01A7-5FEF-41F6-AB65-33675BDDC801}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{123C9D12-8E1A-4AD3-AF3C-541EBD84AAF1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD0D0AC4-5514-4461-83F7-03521B22CAAD}"/>
 </file>
</xml_diff>

<commit_message>
Update to dataset_date & sec_date
</commit_message>
<xml_diff>
--- a/data/_input/base_smartsheet.xlsx
+++ b/data/_input/base_smartsheet.xlsx
@@ -56865,9 +56865,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE9D2FDD-61F1-44F5-AA71-49A169837CE8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BD1AB8A-99E5-48B7-BEB5-B6E63D4168DF}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD0D0AC4-5514-4461-83F7-03521B22CAAD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA005E2A-301F-4A60-BEF5-49209E54543A}"/>
 </file>
</xml_diff>

<commit_message>
Week of 21 July update
</commit_message>
<xml_diff>
--- a/data/_input/base_smartsheet.xlsx
+++ b/data/_input/base_smartsheet.xlsx
@@ -56865,9 +56865,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9BD1AB8A-99E5-48B7-BEB5-B6E63D4168DF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AAB1F98-B12A-4F72-BA16-D3D0DBFAB198}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CA005E2A-301F-4A60-BEF5-49209E54543A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C64C3B28-F3FF-4E18-AF9A-4678A695CAC7}"/>
 </file>
</xml_diff>

<commit_message>
Week of 28 July update
</commit_message>
<xml_diff>
--- a/data/_input/base_smartsheet.xlsx
+++ b/data/_input/base_smartsheet.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31546" uniqueCount="1556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31541" uniqueCount="1556">
   <si>
     <t/>
   </si>
@@ -4862,7 +4862,7 @@
     <numFmt numFmtId="169" formatCode="###0;-###0"/>
     <numFmt numFmtId="170" formatCode="###0.0;-###0.0"/>
   </numFmts>
-  <fonts count="80">
+  <fonts count="86">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -5317,6 +5317,42 @@
     </font>
     <font>
       <name val="Arial"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <color rgb="000000"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <color rgb="000000"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="10.0"/>
+      <color rgb="000000"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="12.0"/>
+      <color rgb="000000"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="Arial"/>
       <sz val="10.0"/>
       <color rgb="000000"/>
       <u val="none"/>
@@ -5346,7 +5382,7 @@
       <u val="none"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5385,6 +5421,16 @@
     </fill>
     <fill>
       <patternFill patternType="none">
+        <fgColor rgb="FEFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FEFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
         <fgColor rgb="C6E7C8"/>
       </patternFill>
     </fill>
@@ -5406,7 +5452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="158">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -5697,28 +5743,52 @@
     <xf numFmtId="168" fontId="73" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
       <alignment horizontal="left" vertical="center" wrapText="false" indent="0"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="74" fillId="9" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true">
+      <alignment horizontal="center" vertical="center" wrapText="true" indent="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="75" fillId="9" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true">
+      <alignment horizontal="center" vertical="center" wrapText="true" indent="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="74" fillId="9" borderId="0" xfId="0" applyFont="true" applyFill="true">
+    <xf numFmtId="0" fontId="76" fillId="9" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment horizontal="center" vertical="center" wrapText="true" indent="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="77" fillId="9" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true">
+      <alignment vertical="top" wrapText="false" indent="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="78" fillId="9" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true">
+      <alignment vertical="top" wrapText="false" indent="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="79" fillId="9" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment vertical="center" wrapText="false" indent="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="80" fillId="11" borderId="0" xfId="0" applyFont="true" applyFill="true">
       <alignment horizontal="left" vertical="center" wrapText="true" indent="0"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="75" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
+    <xf numFmtId="165" fontId="81" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
       <alignment horizontal="left" vertical="center" wrapText="false" indent="0"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
+    <xf numFmtId="166" fontId="82" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
       <alignment horizontal="left" vertical="center" wrapText="false" indent="0"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="77" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
+    <xf numFmtId="166" fontId="83" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
       <alignment horizontal="center" vertical="center" wrapText="true" indent="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="top" wrapText="true" indent="0"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="169" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
+    <xf numFmtId="169" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
       <alignment horizontal="center" vertical="center" wrapText="false" indent="0"/>
     </xf>
   </cellXfs>
@@ -25375,14 +25445,26 @@
         <v>206</v>
       </c>
       <c r="CF77" s="25"/>
-      <c r="CG77" s="111"/>
-      <c r="CH77" s="65"/>
+      <c r="CG77" t="n" s="147">
+        <v>0.7</v>
+      </c>
+      <c r="CH77" t="n" s="149">
+        <v>44742.0</v>
+      </c>
       <c r="CI77" s="61"/>
       <c r="CJ77" s="63"/>
-      <c r="CK77" s="65"/>
-      <c r="CL77" s="113"/>
-      <c r="CM77" s="25"/>
-      <c r="CN77" s="69"/>
+      <c r="CK77" t="s" s="151">
+        <v>207</v>
+      </c>
+      <c r="CL77" t="n" s="153">
+        <v>0.7</v>
+      </c>
+      <c r="CM77" t="n" s="155">
+        <v>44742.0</v>
+      </c>
+      <c r="CN77" t="s" s="157">
+        <v>3</v>
+      </c>
       <c r="CO77" s="71"/>
       <c r="CP77" t="n" s="35">
         <v>0.0</v>
@@ -26714,7 +26796,7 @@
       <c r="CQ82" t="s" s="73">
         <v>206</v>
       </c>
-      <c r="CR82" t="s" s="147">
+      <c r="CR82" t="s" s="159">
         <v>177</v>
       </c>
       <c r="CS82" t="n" s="77">
@@ -30039,10 +30121,10 @@
       <c r="CF96" t="n" s="25">
         <v>2022.0</v>
       </c>
-      <c r="CG96" t="n" s="149">
+      <c r="CG96" t="n" s="161">
         <v>0.7</v>
       </c>
-      <c r="CH96" t="n" s="151">
+      <c r="CH96" t="n" s="163">
         <v>44926.0</v>
       </c>
       <c r="CI96" t="n" s="121">
@@ -34194,7 +34276,7 @@
       <c r="CI112" t="n" s="121">
         <v>0.66</v>
       </c>
-      <c r="CJ112" t="n" s="153">
+      <c r="CJ112" t="n" s="165">
         <v>45291.0</v>
       </c>
       <c r="CK112" t="s" s="65">
@@ -37320,7 +37402,7 @@
         <v>439</v>
       </c>
       <c r="K125" s="3"/>
-      <c r="L125" t="s" s="155">
+      <c r="L125" t="s" s="167">
         <v>227</v>
       </c>
       <c r="M125" s="15"/>
@@ -37328,7 +37410,7 @@
       <c r="O125" s="103"/>
       <c r="P125" s="21"/>
       <c r="Q125" s="23"/>
-      <c r="R125" s="155"/>
+      <c r="R125" s="167"/>
       <c r="S125" s="25"/>
       <c r="T125" s="27"/>
       <c r="U125" s="105"/>
@@ -38160,7 +38242,7 @@
       <c r="CQ128" t="s" s="73">
         <v>313</v>
       </c>
-      <c r="CR128" t="s" s="147">
+      <c r="CR128" t="s" s="159">
         <v>177</v>
       </c>
       <c r="CS128" t="n" s="77">
@@ -46703,14 +46785,24 @@
         <v>206</v>
       </c>
       <c r="CF162" s="25"/>
-      <c r="CG162" s="111"/>
-      <c r="CH162" s="65"/>
+      <c r="CG162" t="n" s="147">
+        <v>0.5</v>
+      </c>
+      <c r="CH162" t="n" s="149">
+        <v>44926.0</v>
+      </c>
       <c r="CI162" s="61"/>
       <c r="CJ162" s="63"/>
       <c r="CK162" s="65"/>
-      <c r="CL162" s="113"/>
-      <c r="CM162" s="25"/>
-      <c r="CN162" s="69"/>
+      <c r="CL162" t="n" s="153">
+        <v>0.5</v>
+      </c>
+      <c r="CM162" t="n" s="155">
+        <v>44926.0</v>
+      </c>
+      <c r="CN162" t="s" s="157">
+        <v>3</v>
+      </c>
       <c r="CO162" s="71"/>
       <c r="CP162" s="47"/>
       <c r="CQ162" t="s" s="73">
@@ -49832,7 +49924,7 @@
       <c r="BG174" s="25"/>
       <c r="BH174" s="25"/>
       <c r="BI174" s="25"/>
-      <c r="BJ174" t="n" s="157">
+      <c r="BJ174" t="n" s="169">
         <v>1058450.0</v>
       </c>
       <c r="BK174" t="n" s="37">
@@ -56656,218 +56748,4 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001F87334A6AC30D4EA6021977FA7E2445" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="504bd14f85abc770ed43885d52246388">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b370a6fa-a798-42e0-969d-19c284d8683f" xmlns:ns3="62ca1376-8bea-4949-825e-fec085c3924e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="823b5556cd3b486fc41cc4ce5ea1e5e3" ns2:_="" ns3:_="">
-    <xsd:import namespace="b370a6fa-a798-42e0-969d-19c284d8683f"/>
-    <xsd:import namespace="62ca1376-8bea-4949-825e-fec085c3924e"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b370a6fa-a798-42e0-969d-19c284d8683f" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="14" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="62ca1376-8bea-4949-825e-fec085c3924e" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="15" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="16" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AAB1F98-B12A-4F72-BA16-D3D0DBFAB198}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C64C3B28-F3FF-4E18-AF9A-4678A695CAC7}"/>
 </file>
</xml_diff>

<commit_message>
Changed input files and dates to reflect pipeline run for week of 220801
</commit_message>
<xml_diff>
--- a/data/_input/base_smartsheet.xlsx
+++ b/data/_input/base_smartsheet.xlsx
@@ -4862,7 +4862,7 @@
     <numFmt numFmtId="169" formatCode="###0;-###0"/>
     <numFmt numFmtId="170" formatCode="###0.0;-###0.0"/>
   </numFmts>
-  <fonts count="86">
+  <fonts count="80">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -5317,42 +5317,6 @@
     </font>
     <font>
       <name val="Arial"/>
-      <sz val="12.0"/>
-      <color rgb="000000"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color rgb="000000"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="000000"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="000000"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="10.0"/>
-      <color rgb="000000"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="12.0"/>
-      <color rgb="000000"/>
-      <u val="none"/>
-    </font>
-    <font>
-      <name val="Arial"/>
       <sz val="10.0"/>
       <color rgb="000000"/>
       <u val="none"/>
@@ -5382,7 +5346,7 @@
       <u val="none"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5421,16 +5385,6 @@
     </fill>
     <fill>
       <patternFill patternType="none">
-        <fgColor rgb="FEFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FEFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
         <fgColor rgb="C6E7C8"/>
       </patternFill>
     </fill>
@@ -5452,7 +5406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="158">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -5743,52 +5697,28 @@
     <xf numFmtId="168" fontId="73" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
       <alignment horizontal="left" vertical="center" wrapText="false" indent="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="74" fillId="9" borderId="0" xfId="0" applyFont="true" applyFill="true">
+      <alignment horizontal="left" vertical="center" wrapText="true" indent="0"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="74" fillId="9" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true">
-      <alignment horizontal="center" vertical="center" wrapText="true" indent="0"/>
+    <xf numFmtId="165" fontId="75" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
+      <alignment horizontal="left" vertical="center" wrapText="false" indent="0"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="75" fillId="9" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true">
+    <xf numFmtId="166" fontId="76" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
+      <alignment horizontal="left" vertical="center" wrapText="false" indent="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="166" fontId="77" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
       <alignment horizontal="center" vertical="center" wrapText="true" indent="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="76" fillId="9" borderId="0" xfId="0" applyFont="true" applyFill="true">
-      <alignment horizontal="center" vertical="center" wrapText="true" indent="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="77" fillId="9" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true">
-      <alignment vertical="top" wrapText="false" indent="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="78" fillId="9" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true">
-      <alignment vertical="top" wrapText="false" indent="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="79" fillId="9" borderId="0" xfId="0" applyFont="true" applyFill="true">
-      <alignment vertical="center" wrapText="false" indent="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="80" fillId="11" borderId="0" xfId="0" applyFont="true" applyFill="true">
-      <alignment horizontal="left" vertical="center" wrapText="true" indent="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="81" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
-      <alignment horizontal="left" vertical="center" wrapText="false" indent="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="82" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
-      <alignment horizontal="left" vertical="center" wrapText="false" indent="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="166" fontId="83" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" wrapText="true" indent="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="84" fillId="0" borderId="0" xfId="0" applyFont="true">
+    <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment vertical="top" wrapText="true" indent="0"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="169" fontId="85" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
+    <xf numFmtId="169" fontId="79" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true">
       <alignment horizontal="center" vertical="center" wrapText="false" indent="0"/>
     </xf>
   </cellXfs>
@@ -25445,24 +25375,24 @@
         <v>206</v>
       </c>
       <c r="CF77" s="25"/>
-      <c r="CG77" t="n" s="147">
+      <c r="CG77" t="n" s="57">
         <v>0.7</v>
       </c>
-      <c r="CH77" t="n" s="149">
+      <c r="CH77" t="n" s="59">
         <v>44742.0</v>
       </c>
       <c r="CI77" s="61"/>
       <c r="CJ77" s="63"/>
-      <c r="CK77" t="s" s="151">
+      <c r="CK77" t="s" s="65">
         <v>207</v>
       </c>
-      <c r="CL77" t="n" s="153">
+      <c r="CL77" t="n" s="67">
         <v>0.7</v>
       </c>
-      <c r="CM77" t="n" s="155">
+      <c r="CM77" t="n" s="41">
         <v>44742.0</v>
       </c>
-      <c r="CN77" t="s" s="157">
+      <c r="CN77" t="s" s="69">
         <v>3</v>
       </c>
       <c r="CO77" s="71"/>
@@ -26796,7 +26726,7 @@
       <c r="CQ82" t="s" s="73">
         <v>206</v>
       </c>
-      <c r="CR82" t="s" s="159">
+      <c r="CR82" t="s" s="147">
         <v>177</v>
       </c>
       <c r="CS82" t="n" s="77">
@@ -30121,10 +30051,10 @@
       <c r="CF96" t="n" s="25">
         <v>2022.0</v>
       </c>
-      <c r="CG96" t="n" s="161">
+      <c r="CG96" t="n" s="149">
         <v>0.7</v>
       </c>
-      <c r="CH96" t="n" s="163">
+      <c r="CH96" t="n" s="151">
         <v>44926.0</v>
       </c>
       <c r="CI96" t="n" s="121">
@@ -34276,7 +34206,7 @@
       <c r="CI112" t="n" s="121">
         <v>0.66</v>
       </c>
-      <c r="CJ112" t="n" s="165">
+      <c r="CJ112" t="n" s="153">
         <v>45291.0</v>
       </c>
       <c r="CK112" t="s" s="65">
@@ -37402,7 +37332,7 @@
         <v>439</v>
       </c>
       <c r="K125" s="3"/>
-      <c r="L125" t="s" s="167">
+      <c r="L125" t="s" s="155">
         <v>227</v>
       </c>
       <c r="M125" s="15"/>
@@ -37410,7 +37340,7 @@
       <c r="O125" s="103"/>
       <c r="P125" s="21"/>
       <c r="Q125" s="23"/>
-      <c r="R125" s="167"/>
+      <c r="R125" s="155"/>
       <c r="S125" s="25"/>
       <c r="T125" s="27"/>
       <c r="U125" s="105"/>
@@ -38242,7 +38172,7 @@
       <c r="CQ128" t="s" s="73">
         <v>313</v>
       </c>
-      <c r="CR128" t="s" s="159">
+      <c r="CR128" t="s" s="147">
         <v>177</v>
       </c>
       <c r="CS128" t="n" s="77">
@@ -46785,22 +46715,22 @@
         <v>206</v>
       </c>
       <c r="CF162" s="25"/>
-      <c r="CG162" t="n" s="147">
+      <c r="CG162" t="n" s="57">
         <v>0.5</v>
       </c>
-      <c r="CH162" t="n" s="149">
+      <c r="CH162" t="n" s="59">
         <v>44926.0</v>
       </c>
       <c r="CI162" s="61"/>
       <c r="CJ162" s="63"/>
       <c r="CK162" s="65"/>
-      <c r="CL162" t="n" s="153">
+      <c r="CL162" t="n" s="67">
         <v>0.5</v>
       </c>
-      <c r="CM162" t="n" s="155">
+      <c r="CM162" t="n" s="41">
         <v>44926.0</v>
       </c>
-      <c r="CN162" t="s" s="157">
+      <c r="CN162" t="s" s="69">
         <v>3</v>
       </c>
       <c r="CO162" s="71"/>
@@ -49924,7 +49854,7 @@
       <c r="BG174" s="25"/>
       <c r="BH174" s="25"/>
       <c r="BI174" s="25"/>
-      <c r="BJ174" t="n" s="169">
+      <c r="BJ174" t="n" s="157">
         <v>1058450.0</v>
       </c>
       <c r="BK174" t="n" s="37">
@@ -56748,4 +56678,218 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001F87334A6AC30D4EA6021977FA7E2445" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="504bd14f85abc770ed43885d52246388">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b370a6fa-a798-42e0-969d-19c284d8683f" xmlns:ns3="62ca1376-8bea-4949-825e-fec085c3924e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="823b5556cd3b486fc41cc4ce5ea1e5e3" ns2:_="" ns3:_="">
+    <xsd:import namespace="b370a6fa-a798-42e0-969d-19c284d8683f"/>
+    <xsd:import namespace="62ca1376-8bea-4949-825e-fec085c3924e"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
+                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="b370a6fa-a798-42e0-969d-19c284d8683f" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="10" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="11" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="13" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="14" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="62ca1376-8bea-4949-825e-fec085c3924e" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="SharedWithUsers" ma:index="15" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:UserMulti">
+            <xsd:sequence>
+              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
+                <xsd:complexType>
+                  <xsd:sequence>
+                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
+                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
+                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
+                  </xsd:sequence>
+                </xsd:complexType>
+              </xsd:element>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="SharedWithDetails" ma:index="16" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED72F416-BC23-4E9E-974A-BE008F2F363A}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56FFC71A-0536-45D3-AA75-6E985B2531D7}"/>
 </file>
</xml_diff>

<commit_message>
New data input files for week of 220815 added
</commit_message>
<xml_diff>
--- a/data/_input/base_smartsheet.xlsx
+++ b/data/_input/base_smartsheet.xlsx
@@ -56681,8 +56681,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001F87334A6AC30D4EA6021977FA7E2445" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="504bd14f85abc770ed43885d52246388">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b370a6fa-a798-42e0-969d-19c284d8683f" xmlns:ns3="62ca1376-8bea-4949-825e-fec085c3924e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="823b5556cd3b486fc41cc4ce5ea1e5e3" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001F87334A6AC30D4EA6021977FA7E2445" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="13eff9136b4917bb459ad9c1db870f6d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b370a6fa-a798-42e0-969d-19c284d8683f" xmlns:ns3="62ca1376-8bea-4949-825e-fec085c3924e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60e7197df19c7150b1ba0c3bfe00adf4" ns2:_="" ns3:_="">
     <xsd:import namespace="b370a6fa-a798-42e0-969d-19c284d8683f"/>
     <xsd:import namespace="62ca1376-8bea-4949-825e-fec085c3924e"/>
     <xsd:element name="properties">
@@ -56700,6 +56700,9 @@
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -56745,6 +56748,23 @@
     <xsd:element name="MediaLengthInSeconds" ma:index="14" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="18" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="19" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="20" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -56887,9 +56907,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D56B283-4A56-4143-A018-ECECC59CE994}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F355051-25BF-4A67-A824-5EAF2851BD41}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DA73A51-DAC7-4DDF-A32F-95473C2CF03B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5817531B-D928-4096-A5BE-7FED91362A84}"/>
 </file>
</xml_diff>